<commit_message>
zapocete promene na json datotekama da budu csv
</commit_message>
<xml_diff>
--- a/Zahtevi.xlsx
+++ b/Zahtevi.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F1398C-899C-4AAD-B059-C25460FA4E73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22332" windowHeight="12048"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="52">
   <si>
     <t>Opis</t>
   </si>
@@ -50,18 +49,12 @@
     <t>Funkcionalni</t>
   </si>
   <si>
-    <t>1.4.1</t>
-  </si>
-  <si>
     <t>Obezbediti kreiranje i preuzimanje informacionih resursa.</t>
   </si>
   <si>
     <t>Obezbediti mogućnost izmene, kreiranja, brisanja, pretrage i prikaza informacionih resursa.</t>
   </si>
   <si>
-    <t>Obezbediti u prikazu mogućnost sortiranja informacionih resursa.</t>
-  </si>
-  <si>
     <t>Obezbediti mogućnost izmene, kreiranja, brisanja, pretrage i prikaza elemenata informacionih resursa.</t>
   </si>
   <si>
@@ -104,9 +97,6 @@
     <t>Obezbediti da su razdvojeni struktura informacionih resursa i model prikaza informacionih resursa</t>
   </si>
   <si>
-    <t>Obezbediti rukovanje sa različitim tipovima informacionih resursa. Pod informacionim resursom podrazumevamo podatke, informacije, znanje i inteligenciju.</t>
-  </si>
-  <si>
     <t>Administrator informacionih resursa</t>
   </si>
   <si>
@@ -174,12 +164,18 @@
   </si>
   <si>
     <t>Administrator alata, Administrator informacionih resursa, Operativni korisnik</t>
+  </si>
+  <si>
+    <t>Obezbediti rukovanje sa različitim tipovima informacionih resursa. Pod informacionim resursom podrazumevamo podatke, informacije, znanje i mudrost.</t>
+  </si>
+  <si>
+    <t>zahtev na 1h:14m 10.12.2020 prvi cas sort datoteke</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,23 +409,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -465,23 +444,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -657,27 +619,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.796875" defaultRowHeight="50" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="49.95" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.8984375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="36.69921875" style="6" customWidth="1"/>
-    <col min="3" max="4" width="15.796875" style="1"/>
-    <col min="5" max="5" width="35.69921875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="15.796875" style="1"/>
-    <col min="8" max="8" width="18.3984375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="15.796875" style="3"/>
+    <col min="1" max="1" width="14.88671875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="15.77734375" style="1"/>
+    <col min="5" max="5" width="35.6640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.77734375" style="1"/>
+    <col min="8" max="8" width="18.44140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="15.77734375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -703,7 +665,7 @@
     </row>
     <row r="2" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -716,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -725,7 +687,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
@@ -742,7 +704,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -751,7 +713,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
@@ -768,7 +730,7 @@
         <v>1.2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -777,7 +739,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -794,7 +756,7 @@
         <v>1.3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -803,7 +765,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>7</v>
@@ -820,7 +782,7 @@
         <v>1.4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -829,7 +791,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>7</v>
@@ -842,11 +804,11 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>11</v>
+      <c r="A8" s="8">
+        <v>2</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -855,7 +817,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>7</v>
@@ -868,42 +830,42 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
-        <v>2</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="2">
-        <v>7</v>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
-        <v>18</v>
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>10</v>
@@ -912,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>7</v>
@@ -926,10 +888,10 @@
     </row>
     <row r="12" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
@@ -938,7 +900,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>7</v>
@@ -951,11 +913,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8">
-        <v>3.2</v>
+      <c r="A13" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>10</v>
@@ -964,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>7</v>
@@ -977,11 +939,11 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>27</v>
+      <c r="A14" s="8">
+        <v>4</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>10</v>
@@ -990,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>7</v>
@@ -1003,73 +965,73 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
-        <v>4</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="2">
-        <v>7</v>
+      <c r="B15" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="9" t="s">
-        <v>33</v>
+      <c r="A16" s="8">
+        <v>5</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
-        <v>5</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="2">
-        <v>7</v>
+      <c r="B17" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="8">
+        <v>6</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
-        <v>6</v>
+        <v>6.1</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
@@ -1078,7 +1040,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -1092,10 +1054,10 @@
     </row>
     <row r="20" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
-        <v>6.1</v>
+        <v>7</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>10</v>
@@ -1118,10 +1080,10 @@
     </row>
     <row r="21" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>10</v>
@@ -1130,7 +1092,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>7</v>
@@ -1144,10 +1106,10 @@
     </row>
     <row r="22" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
@@ -1156,7 +1118,7 @@
         <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>7</v>
@@ -1170,19 +1132,19 @@
     </row>
     <row r="23" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>7</v>
@@ -1195,77 +1157,74 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8">
-        <v>10</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
+        <v>11</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
+      <c r="E25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>12</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="8">
-        <v>11</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
-        <v>12</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>7</v>
@@ -1274,37 +1233,20 @@
         <v>8</v>
       </c>
       <c r="H27" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="64.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
dodavanje use case dijagrama
</commit_message>
<xml_diff>
--- a/Zahtevi.xlsx
+++ b/Zahtevi.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_3E14E5DFB9AC2D59A5589D8200BF18131DB02DDC" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C953305E-3069-48BB-85E9-01A2AC9AC0B3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22332" windowHeight="12048"/>
+    <workbookView xWindow="11935" yWindow="4205" windowWidth="16589" windowHeight="8582" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,6 +410,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -444,6 +462,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,22 +654,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="49.95" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.796875" defaultRowHeight="50" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.77734375" style="8"/>
-    <col min="5" max="5" width="35.6640625" style="8" customWidth="1"/>
-    <col min="6" max="7" width="15.77734375" style="8"/>
-    <col min="8" max="8" width="18.44140625" style="9" customWidth="1"/>
-    <col min="9" max="16384" width="15.77734375" style="7"/>
+    <col min="1" max="1" width="14.8984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.69921875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.796875" style="8"/>
+    <col min="5" max="5" width="35.69921875" style="8" customWidth="1"/>
+    <col min="6" max="7" width="15.796875" style="8"/>
+    <col min="8" max="8" width="18.3984375" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="15.796875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1125,29 +1160,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="64.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:8" ht="64.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>